<commit_message>
C01-Enhancements: -Table responsive -Loading indicator
</commit_message>
<xml_diff>
--- a/src/assets/data/lista de precios 14-01-22.xlsx
+++ b/src/assets/data/lista de precios 14-01-22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\centralia-web\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE94F8C-494E-41FD-B3B6-4F57C74ED40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4BAE4C-329B-42A3-A280-7A96F2461E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -8899,13 +8899,11 @@
   </sheetPr>
   <dimension ref="A1:D1438"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C194" sqref="C194:C217"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="35" style="2" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="2" customWidth="1"/>
@@ -8926,7 +8924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1795</v>
       </c>
@@ -8940,7 +8938,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1798</v>
       </c>
@@ -8954,7 +8952,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1800</v>
       </c>
@@ -8968,7 +8966,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1802</v>
       </c>
@@ -8982,7 +8980,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>1804</v>
       </c>
@@ -8996,7 +8994,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>1806</v>
       </c>
@@ -9010,7 +9008,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1808</v>
       </c>
@@ -9024,7 +9022,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1810</v>
       </c>
@@ -9038,7 +9036,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1812</v>
       </c>
@@ -9052,7 +9050,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1814</v>
       </c>
@@ -9066,7 +9064,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1816</v>
       </c>
@@ -9080,7 +9078,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>1818</v>
       </c>
@@ -9094,7 +9092,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>1820</v>
       </c>
@@ -9108,7 +9106,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>1822</v>
       </c>
@@ -9122,7 +9120,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>1824</v>
       </c>
@@ -9136,7 +9134,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>1826</v>
       </c>
@@ -9150,7 +9148,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>1828</v>
       </c>
@@ -9164,7 +9162,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>1830</v>
       </c>
@@ -9178,7 +9176,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>1832</v>
       </c>
@@ -9192,7 +9190,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>1834</v>
       </c>
@@ -9206,7 +9204,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>1836</v>
       </c>
@@ -9220,7 +9218,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>1838</v>
       </c>
@@ -9234,7 +9232,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>1840</v>
       </c>
@@ -9248,7 +9246,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>1842</v>
       </c>
@@ -9262,7 +9260,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>1844</v>
       </c>
@@ -9276,7 +9274,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>1846</v>
       </c>
@@ -9290,7 +9288,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>1848</v>
       </c>
@@ -9304,7 +9302,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>1850</v>
       </c>
@@ -9318,7 +9316,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>1852</v>
       </c>
@@ -9332,7 +9330,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>1854</v>
       </c>
@@ -9346,7 +9344,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>1856</v>
       </c>
@@ -9360,7 +9358,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>1858</v>
       </c>
@@ -9374,7 +9372,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>1860</v>
       </c>
@@ -9388,7 +9386,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>1862</v>
       </c>
@@ -9402,7 +9400,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>1864</v>
       </c>
@@ -9416,7 +9414,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>1866</v>
       </c>
@@ -9430,7 +9428,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>1868</v>
       </c>
@@ -9444,7 +9442,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>1870</v>
       </c>
@@ -9458,7 +9456,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>1872</v>
       </c>
@@ -9472,7 +9470,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>1874</v>
       </c>
@@ -9486,7 +9484,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>1876</v>
       </c>
@@ -9500,7 +9498,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>1878</v>
       </c>
@@ -9514,7 +9512,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>1880</v>
       </c>
@@ -9528,7 +9526,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>1882</v>
       </c>
@@ -9542,7 +9540,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>1884</v>
       </c>
@@ -9556,7 +9554,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>1886</v>
       </c>
@@ -9570,7 +9568,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>1888</v>
       </c>
@@ -9584,7 +9582,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>1890</v>
       </c>
@@ -9598,7 +9596,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>1892</v>
       </c>
@@ -9612,7 +9610,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>1894</v>
       </c>
@@ -9626,7 +9624,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>1896</v>
       </c>
@@ -9640,7 +9638,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>1898</v>
       </c>
@@ -9654,7 +9652,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>1900</v>
       </c>
@@ -9668,7 +9666,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>1902</v>
       </c>
@@ -9682,7 +9680,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>1904</v>
       </c>
@@ -9696,7 +9694,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>1906</v>
       </c>
@@ -9710,7 +9708,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>1908</v>
       </c>
@@ -9724,7 +9722,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>1910</v>
       </c>
@@ -9738,7 +9736,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>1912</v>
       </c>
@@ -9752,7 +9750,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>1914</v>
       </c>
@@ -9766,7 +9764,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>1916</v>
       </c>
@@ -9780,7 +9778,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>1918</v>
       </c>
@@ -9794,7 +9792,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>1920</v>
       </c>
@@ -9808,7 +9806,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>1922</v>
       </c>
@@ -9822,7 +9820,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>1924</v>
       </c>
@@ -9836,7 +9834,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>1926</v>
       </c>
@@ -9850,7 +9848,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>1928</v>
       </c>
@@ -9864,7 +9862,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>1930</v>
       </c>
@@ -9878,7 +9876,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>1932</v>
       </c>
@@ -9892,7 +9890,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>1934</v>
       </c>
@@ -9906,7 +9904,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>1936</v>
       </c>
@@ -9920,7 +9918,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>1938</v>
       </c>
@@ -9934,7 +9932,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>1940</v>
       </c>
@@ -9948,7 +9946,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>1942</v>
       </c>
@@ -9962,7 +9960,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>1944</v>
       </c>
@@ -9976,7 +9974,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>1946</v>
       </c>
@@ -9990,7 +9988,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>1948</v>
       </c>
@@ -10004,7 +10002,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>1950</v>
       </c>
@@ -10018,7 +10016,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>1952</v>
       </c>
@@ -10032,7 +10030,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>1954</v>
       </c>
@@ -10046,7 +10044,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>1956</v>
       </c>
@@ -10060,7 +10058,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>1958</v>
       </c>
@@ -10074,7 +10072,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>1960</v>
       </c>
@@ -10088,7 +10086,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>1962</v>
       </c>
@@ -10102,7 +10100,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>1964</v>
       </c>
@@ -10116,7 +10114,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>1966</v>
       </c>
@@ -10130,7 +10128,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>1968</v>
       </c>
@@ -10144,7 +10142,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>1970</v>
       </c>
@@ -10158,7 +10156,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>1972</v>
       </c>
@@ -10172,7 +10170,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>1974</v>
       </c>
@@ -10186,7 +10184,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>1976</v>
       </c>
@@ -10200,7 +10198,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>1978</v>
       </c>
@@ -10214,7 +10212,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>1980</v>
       </c>
@@ -10228,7 +10226,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>1982</v>
       </c>
@@ -10242,7 +10240,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>1984</v>
       </c>
@@ -10256,7 +10254,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>1986</v>
       </c>
@@ -10270,7 +10268,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>1988</v>
       </c>
@@ -10284,7 +10282,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>1990</v>
       </c>
@@ -10298,7 +10296,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>1992</v>
       </c>
@@ -10312,7 +10310,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>1994</v>
       </c>
@@ -10326,7 +10324,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>1996</v>
       </c>
@@ -10340,7 +10338,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>1998</v>
       </c>
@@ -10354,7 +10352,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>2000</v>
       </c>
@@ -10368,7 +10366,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>2002</v>
       </c>
@@ -10382,7 +10380,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>2004</v>
       </c>
@@ -10396,7 +10394,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>2006</v>
       </c>
@@ -10410,7 +10408,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>2008</v>
       </c>
@@ -10424,7 +10422,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>2010</v>
       </c>
@@ -10438,7 +10436,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>2012</v>
       </c>
@@ -10452,7 +10450,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>2014</v>
       </c>
@@ -10466,7 +10464,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>2016</v>
       </c>
@@ -10480,7 +10478,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>2018</v>
       </c>
@@ -10494,7 +10492,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>2020</v>
       </c>
@@ -10508,7 +10506,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>2022</v>
       </c>
@@ -10522,7 +10520,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>2024</v>
       </c>
@@ -10536,7 +10534,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>2026</v>
       </c>
@@ -10550,7 +10548,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>2028</v>
       </c>
@@ -10564,7 +10562,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>2030</v>
       </c>
@@ -10578,7 +10576,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>2032</v>
       </c>
@@ -10592,7 +10590,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>2034</v>
       </c>
@@ -10606,7 +10604,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>2036</v>
       </c>
@@ -10620,7 +10618,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>2038</v>
       </c>
@@ -10634,7 +10632,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>2040</v>
       </c>
@@ -10648,7 +10646,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>2042</v>
       </c>
@@ -10662,7 +10660,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>2044</v>
       </c>
@@ -10676,7 +10674,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>2046</v>
       </c>
@@ -10690,7 +10688,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>2048</v>
       </c>
@@ -10704,7 +10702,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>2050</v>
       </c>
@@ -10718,7 +10716,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>2052</v>
       </c>
@@ -10732,7 +10730,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>2054</v>
       </c>
@@ -10746,7 +10744,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>2056</v>
       </c>
@@ -10760,7 +10758,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>2058</v>
       </c>
@@ -10774,7 +10772,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>2060</v>
       </c>
@@ -10788,7 +10786,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>2062</v>
       </c>
@@ -10802,7 +10800,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>2064</v>
       </c>
@@ -10816,7 +10814,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>2066</v>
       </c>
@@ -10830,7 +10828,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>2068</v>
       </c>
@@ -10844,7 +10842,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>2070</v>
       </c>
@@ -10858,7 +10856,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>2072</v>
       </c>
@@ -10872,7 +10870,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>2074</v>
       </c>
@@ -10886,7 +10884,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>2076</v>
       </c>
@@ -10900,7 +10898,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>2078</v>
       </c>
@@ -10914,7 +10912,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>2080</v>
       </c>
@@ -10928,7 +10926,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>2082</v>
       </c>
@@ -10942,7 +10940,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>2084</v>
       </c>
@@ -10956,7 +10954,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>2086</v>
       </c>
@@ -10970,7 +10968,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>2088</v>
       </c>
@@ -10984,7 +10982,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>2090</v>
       </c>
@@ -10998,7 +10996,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>2092</v>
       </c>
@@ -11012,7 +11010,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>2094</v>
       </c>
@@ -11026,7 +11024,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>2096</v>
       </c>
@@ -11040,7 +11038,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>2098</v>
       </c>
@@ -11054,7 +11052,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>2100</v>
       </c>
@@ -11068,7 +11066,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>2102</v>
       </c>
@@ -11082,7 +11080,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>2104</v>
       </c>
@@ -11096,7 +11094,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>2106</v>
       </c>
@@ -11110,7 +11108,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>2108</v>
       </c>
@@ -11124,7 +11122,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>2110</v>
       </c>
@@ -11138,7 +11136,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>2112</v>
       </c>
@@ -11152,7 +11150,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>2114</v>
       </c>
@@ -11166,7 +11164,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>2116</v>
       </c>
@@ -11180,7 +11178,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>2118</v>
       </c>
@@ -11194,7 +11192,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>2120</v>
       </c>
@@ -11614,7 +11612,7 @@
         <v>2687</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>2379</v>
       </c>
@@ -11628,7 +11626,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>2382</v>
       </c>
@@ -11642,7 +11640,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>2384</v>
       </c>
@@ -11656,7 +11654,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>2386</v>
       </c>
@@ -11670,7 +11668,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>2388</v>
       </c>
@@ -11684,7 +11682,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>2390</v>
       </c>
@@ -11698,7 +11696,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>2392</v>
       </c>
@@ -11712,7 +11710,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>2394</v>
       </c>
@@ -11726,7 +11724,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>2396</v>
       </c>
@@ -11740,7 +11738,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>2398</v>
       </c>
@@ -11754,7 +11752,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>2400</v>
       </c>
@@ -11768,7 +11766,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>2402</v>
       </c>
@@ -11782,7 +11780,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>2404</v>
       </c>
@@ -11796,7 +11794,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>2405</v>
       </c>
@@ -11810,7 +11808,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>2407</v>
       </c>
@@ -11824,7 +11822,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>2409</v>
       </c>
@@ -11838,7 +11836,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>2411</v>
       </c>
@@ -11852,7 +11850,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>2413</v>
       </c>
@@ -11866,7 +11864,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>2415</v>
       </c>
@@ -11880,7 +11878,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>2417</v>
       </c>
@@ -11894,7 +11892,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>2419</v>
       </c>
@@ -11908,7 +11906,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>2421</v>
       </c>
@@ -11922,7 +11920,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>2423</v>
       </c>
@@ -11936,7 +11934,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>2425</v>
       </c>
@@ -29048,7 +29046,7 @@
   <autoFilter ref="A1:D1438" xr:uid="{C920CB92-BC7E-4103-9DA8-5ADCA6570DC2}">
     <filterColumn colId="3">
       <filters>
-        <filter val="030 POLVOS PARA AGUAS"/>
+        <filter val="010 LIMPIADORES"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>